<commit_message>
added all postag for TX.
</commit_message>
<xml_diff>
--- a/output/TXTX.xlsx
+++ b/output/TXTX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1B78577-C0DF-40FD-8CA9-983714D1D010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7721D8B-4532-4CA9-AAFB-5CCA77BD0D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15225" windowHeight="13605" activeTab="9" xr2:uid="{9BDD03C8-F7C5-4674-9603-EB57B3FD651B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9BDD03C8-F7C5-4674-9603-EB57B3FD651B}"/>
   </bookViews>
   <sheets>
     <sheet name="BOW1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <sheet name="DICTTFIDF" sheetId="6" r:id="rId8"/>
     <sheet name="W2V_AVG" sheetId="8" r:id="rId9"/>
     <sheet name="W2V_TF" sheetId="11" r:id="rId10"/>
-    <sheet name="POSTAG" sheetId="7" r:id="rId11"/>
+    <sheet name="POSTAG-BOW" sheetId="7" r:id="rId11"/>
+    <sheet name="POSTAG-AVG" sheetId="13" r:id="rId12"/>
+    <sheet name="POSTAG-CONCAT" sheetId="12" r:id="rId13"/>
+    <sheet name="POSTAG-FLAT" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="1366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="1817">
   <si>
     <t>SVM</t>
   </si>
@@ -4143,6 +4146,1359 @@
   </si>
   <si>
     <t>0.623±0.624</t>
+  </si>
+  <si>
+    <t>0.6124±0.0012</t>
+  </si>
+  <si>
+    <t>0.3062±0.0006</t>
+  </si>
+  <si>
+    <t>0.5±0.0</t>
+  </si>
+  <si>
+    <t>0.0±0.0</t>
+  </si>
+  <si>
+    <t>0.3798±0.0005</t>
+  </si>
+  <si>
+    <t>0.5675±0.0947</t>
+  </si>
+  <si>
+    <t>0.2838±0.0474</t>
+  </si>
+  <si>
+    <t>0.3598±0.0423</t>
+  </si>
+  <si>
+    <t>0.5458±0.1082</t>
+  </si>
+  <si>
+    <t>0.2729±0.0541</t>
+  </si>
+  <si>
+    <t>0.3501±0.0483</t>
+  </si>
+  <si>
+    <t>0.4551±0.1086</t>
+  </si>
+  <si>
+    <t>0.2276±0.0543</t>
+  </si>
+  <si>
+    <t>0.3095±0.0486</t>
+  </si>
+  <si>
+    <t>0.5005±0.1185</t>
+  </si>
+  <si>
+    <t>0.2502±0.0592</t>
+  </si>
+  <si>
+    <t>0.499±0.0022</t>
+  </si>
+  <si>
+    <t>0.3298±0.0529</t>
+  </si>
+  <si>
+    <t>0.5897±0.0714</t>
+  </si>
+  <si>
+    <t>0.2949±0.0357</t>
+  </si>
+  <si>
+    <t>0.3697±0.0319</t>
+  </si>
+  <si>
+    <t>0.6119±0.0012</t>
+  </si>
+  <si>
+    <t>0.306±0.0006</t>
+  </si>
+  <si>
+    <t>0.3796±0.0005</t>
+  </si>
+  <si>
+    <t>0.5001±0.0003</t>
+  </si>
+  <si>
+    <t>0.5897±0.0705</t>
+  </si>
+  <si>
+    <t>0.2949±0.0353</t>
+  </si>
+  <si>
+    <t>0.3697±0.0315</t>
+  </si>
+  <si>
+    <t>0.5757±0.0364</t>
+  </si>
+  <si>
+    <t>0.5732±0.0353</t>
+  </si>
+  <si>
+    <t>0.5736±0.0362</t>
+  </si>
+  <si>
+    <t>0.1468±0.0714</t>
+  </si>
+  <si>
+    <t>0.6016±0.0388</t>
+  </si>
+  <si>
+    <t>0.5986±0.0371</t>
+  </si>
+  <si>
+    <t>0.5803±0.0454</t>
+  </si>
+  <si>
+    <t>0.5645±0.0387</t>
+  </si>
+  <si>
+    <t>0.1429±0.0805</t>
+  </si>
+  <si>
+    <t>0.5911±0.0456</t>
+  </si>
+  <si>
+    <t>0.5513±0.0388</t>
+  </si>
+  <si>
+    <t>0.5721±0.0272</t>
+  </si>
+  <si>
+    <t>0.5704±0.0289</t>
+  </si>
+  <si>
+    <t>0.1424±0.0558</t>
+  </si>
+  <si>
+    <t>0.5957±0.0429</t>
+  </si>
+  <si>
+    <t>0.5666±0.0432</t>
+  </si>
+  <si>
+    <t>0.5769±0.03</t>
+  </si>
+  <si>
+    <t>0.5767±0.0306</t>
+  </si>
+  <si>
+    <t>0.1535±0.0603</t>
+  </si>
+  <si>
+    <t>0.5981±0.0394</t>
+  </si>
+  <si>
+    <t>0.51±0.0316</t>
+  </si>
+  <si>
+    <t>0.5802±0.031</t>
+  </si>
+  <si>
+    <t>0.5639±0.0252</t>
+  </si>
+  <si>
+    <t>0.1427±0.0547</t>
+  </si>
+  <si>
+    <t>0.5928±0.0303</t>
+  </si>
+  <si>
+    <t>0.5511±0.0276</t>
+  </si>
+  <si>
+    <t>0.5682±0.0169</t>
+  </si>
+  <si>
+    <t>0.568±0.018</t>
+  </si>
+  <si>
+    <t>0.1361±0.0346</t>
+  </si>
+  <si>
+    <t>0.5904±0.027</t>
+  </si>
+  <si>
+    <t>0.5671±0.0311</t>
+  </si>
+  <si>
+    <t>0.5833±0.0285</t>
+  </si>
+  <si>
+    <t>0.5839±0.0273</t>
+  </si>
+  <si>
+    <t>0.1672±0.0555</t>
+  </si>
+  <si>
+    <t>0.6046±0.0354</t>
+  </si>
+  <si>
+    <t>0.5919±0.0476</t>
+  </si>
+  <si>
+    <t>0.5705±0.0455</t>
+  </si>
+  <si>
+    <t>0.5327±0.0213</t>
+  </si>
+  <si>
+    <t>0.0929±0.0525</t>
+  </si>
+  <si>
+    <t>0.5767±0.0491</t>
+  </si>
+  <si>
+    <t>0.532±0.0444</t>
+  </si>
+  <si>
+    <t>0.5363±0.0316</t>
+  </si>
+  <si>
+    <t>0.5337±0.0284</t>
+  </si>
+  <si>
+    <t>0.0698±0.0593</t>
+  </si>
+  <si>
+    <t>0.5193±0.0324</t>
+  </si>
+  <si>
+    <t>0.5415±0.0338</t>
+  </si>
+  <si>
+    <t>0.5394±0.0335</t>
+  </si>
+  <si>
+    <t>0.0808±0.0671</t>
+  </si>
+  <si>
+    <t>0.6241±0.012</t>
+  </si>
+  <si>
+    <t>0.5577±0.1912</t>
+  </si>
+  <si>
+    <t>0.5315±0.0315</t>
+  </si>
+  <si>
+    <t>0.0978±0.0762</t>
+  </si>
+  <si>
+    <t>0.5953±0.043</t>
+  </si>
+  <si>
+    <t>0.6014±0.0398</t>
+  </si>
+  <si>
+    <t>0.5791±0.0486</t>
+  </si>
+  <si>
+    <t>0.5674±0.0403</t>
+  </si>
+  <si>
+    <t>0.1453±0.0864</t>
+  </si>
+  <si>
+    <t>0.6063±0.0372</t>
+  </si>
+  <si>
+    <t>0.5734±0.0357</t>
+  </si>
+  <si>
+    <t>0.5721±0.0405</t>
+  </si>
+  <si>
+    <t>0.5713±0.0279</t>
+  </si>
+  <si>
+    <t>0.5768±0.0302</t>
+  </si>
+  <si>
+    <t>0.5719±0.0274</t>
+  </si>
+  <si>
+    <t>0.5681±0.0173</t>
+  </si>
+  <si>
+    <t>0.5836±0.0278</t>
+  </si>
+  <si>
+    <t>0.5504±0.0284</t>
+  </si>
+  <si>
+    <t>0.535±0.0297</t>
+  </si>
+  <si>
+    <t>0.5405±0.0336</t>
+  </si>
+  <si>
+    <t>0.5301±0.1053</t>
+  </si>
+  <si>
+    <t>0.5731±0.0435</t>
+  </si>
+  <si>
+    <t>0.6196±0.0208</t>
+  </si>
+  <si>
+    <t>0.5865±0.0398</t>
+  </si>
+  <si>
+    <t>0.5447±0.0231</t>
+  </si>
+  <si>
+    <t>0.1225±0.0554</t>
+  </si>
+  <si>
+    <t>0.5975±0.0335</t>
+  </si>
+  <si>
+    <t>0.5645±0.0284</t>
+  </si>
+  <si>
+    <t>0.6043±0.0193</t>
+  </si>
+  <si>
+    <t>0.569±0.025</t>
+  </si>
+  <si>
+    <t>0.5552±0.0198</t>
+  </si>
+  <si>
+    <t>0.1231±0.0431</t>
+  </si>
+  <si>
+    <t>0.6067±0.0293</t>
+  </si>
+  <si>
+    <t>0.562±0.0217</t>
+  </si>
+  <si>
+    <t>0.5814±0.0283</t>
+  </si>
+  <si>
+    <t>0.5493±0.03</t>
+  </si>
+  <si>
+    <t>0.5454±0.0288</t>
+  </si>
+  <si>
+    <t>0.0945±0.0587</t>
+  </si>
+  <si>
+    <t>0.5677±0.0337</t>
+  </si>
+  <si>
+    <t>0.5473±0.0293</t>
+  </si>
+  <si>
+    <t>0.5742±0.0256</t>
+  </si>
+  <si>
+    <t>0.5465±0.0238</t>
+  </si>
+  <si>
+    <t>0.5439±0.0217</t>
+  </si>
+  <si>
+    <t>0.0903±0.0454</t>
+  </si>
+  <si>
+    <t>0.5577±0.0288</t>
+  </si>
+  <si>
+    <t>0.5452±0.0227</t>
+  </si>
+  <si>
+    <t>0.6062±0.0187</t>
+  </si>
+  <si>
+    <t>0.5777±0.0184</t>
+  </si>
+  <si>
+    <t>0.5699±0.0169</t>
+  </si>
+  <si>
+    <t>0.1473±0.0342</t>
+  </si>
+  <si>
+    <t>0.6166±0.0235</t>
+  </si>
+  <si>
+    <t>0.5738±0.0171</t>
+  </si>
+  <si>
+    <t>0.5921±0.0254</t>
+  </si>
+  <si>
+    <t>0.5621±0.028</t>
+  </si>
+  <si>
+    <t>0.5576±0.0272</t>
+  </si>
+  <si>
+    <t>0.1195±0.055</t>
+  </si>
+  <si>
+    <t>0.5938±0.0312</t>
+  </si>
+  <si>
+    <t>0.5598±0.0275</t>
+  </si>
+  <si>
+    <t>0.5668±0.0311</t>
+  </si>
+  <si>
+    <t>0.5419±0.0311</t>
+  </si>
+  <si>
+    <t>0.5409±0.0302</t>
+  </si>
+  <si>
+    <t>0.0827±0.0612</t>
+  </si>
+  <si>
+    <t>0.5754±0.0293</t>
+  </si>
+  <si>
+    <t>0.5414±0.0306</t>
+  </si>
+  <si>
+    <t>0.5814±0.06</t>
+  </si>
+  <si>
+    <t>0.5535±0.0438</t>
+  </si>
+  <si>
+    <t>0.5219±0.0238</t>
+  </si>
+  <si>
+    <t>0.0655±0.055</t>
+  </si>
+  <si>
+    <t>0.5803±0.0332</t>
+  </si>
+  <si>
+    <t>0.5368±0.0299</t>
+  </si>
+  <si>
+    <t>0.5327±0.0293</t>
+  </si>
+  <si>
+    <t>0.5197±0.029</t>
+  </si>
+  <si>
+    <t>0.5202±0.0292</t>
+  </si>
+  <si>
+    <t>0.0399±0.0581</t>
+  </si>
+  <si>
+    <t>0.52±0.0291</t>
+  </si>
+  <si>
+    <t>0.5453±0.0255</t>
+  </si>
+  <si>
+    <t>0.5311±0.0223</t>
+  </si>
+  <si>
+    <t>0.5319±0.023</t>
+  </si>
+  <si>
+    <t>0.063±0.0453</t>
+  </si>
+  <si>
+    <t>0.5372±0.0298</t>
+  </si>
+  <si>
+    <t>0.5315±0.0226</t>
+  </si>
+  <si>
+    <t>0.6117±0.0176</t>
+  </si>
+  <si>
+    <t>0.4871±0.1376</t>
+  </si>
+  <si>
+    <t>0.5126±0.0251</t>
+  </si>
+  <si>
+    <t>0.0418±0.0715</t>
+  </si>
+  <si>
+    <t>0.6135±0.0317</t>
+  </si>
+  <si>
+    <t>0.4913±0.0851</t>
+  </si>
+  <si>
+    <t>0.622±0.0236</t>
+  </si>
+  <si>
+    <t>0.5902±0.0433</t>
+  </si>
+  <si>
+    <t>0.5568±0.0264</t>
+  </si>
+  <si>
+    <t>0.1419±0.063</t>
+  </si>
+  <si>
+    <t>0.6206±0.0307</t>
+  </si>
+  <si>
+    <t>0.5727±0.0323</t>
+  </si>
+  <si>
+    <t>0.6556±0.016</t>
+  </si>
+  <si>
+    <t>0.634±0.0189</t>
+  </si>
+  <si>
+    <t>0.6097±0.0273</t>
+  </si>
+  <si>
+    <t>0.2416±0.0459</t>
+  </si>
+  <si>
+    <t>0.6624±0.0305</t>
+  </si>
+  <si>
+    <t>0.6215±0.022</t>
+  </si>
+  <si>
+    <t>0.6434±0.0302</t>
+  </si>
+  <si>
+    <t>0.624±0.0335</t>
+  </si>
+  <si>
+    <t>0.609±0.0351</t>
+  </si>
+  <si>
+    <t>0.2322±0.068</t>
+  </si>
+  <si>
+    <t>0.6611±0.0308</t>
+  </si>
+  <si>
+    <t>0.6164±0.0339</t>
+  </si>
+  <si>
+    <t>0.6069±0.0298</t>
+  </si>
+  <si>
+    <t>0.6257±0.0271</t>
+  </si>
+  <si>
+    <t>0.6267±0.0256</t>
+  </si>
+  <si>
+    <t>0.2523±0.052</t>
+  </si>
+  <si>
+    <t>0.6752±0.033</t>
+  </si>
+  <si>
+    <t>0.6262±0.026</t>
+  </si>
+  <si>
+    <t>0.6382±0.0207</t>
+  </si>
+  <si>
+    <t>0.622±0.0235</t>
+  </si>
+  <si>
+    <t>0.6227±0.0258</t>
+  </si>
+  <si>
+    <t>0.2446±0.049</t>
+  </si>
+  <si>
+    <t>0.6646±0.0325</t>
+  </si>
+  <si>
+    <t>0.6223±0.0245</t>
+  </si>
+  <si>
+    <t>0.6253±0.0251</t>
+  </si>
+  <si>
+    <t>0.614±0.0216</t>
+  </si>
+  <si>
+    <t>0.6097±0.0258</t>
+  </si>
+  <si>
+    <t>0.2231±0.0449</t>
+  </si>
+  <si>
+    <t>0.6638±0.0362</t>
+  </si>
+  <si>
+    <t>0.6117±0.0224</t>
+  </si>
+  <si>
+    <t>0.5754±0.0274</t>
+  </si>
+  <si>
+    <t>0.614±0.0273</t>
+  </si>
+  <si>
+    <t>0.608±0.0242</t>
+  </si>
+  <si>
+    <t>0.2217±0.0501</t>
+  </si>
+  <si>
+    <t>0.6575±0.0428</t>
+  </si>
+  <si>
+    <t>0.6109±0.0251</t>
+  </si>
+  <si>
+    <t>0.6494±0.0215</t>
+  </si>
+  <si>
+    <t>0.6333±0.0229</t>
+  </si>
+  <si>
+    <t>0.6312±0.0243</t>
+  </si>
+  <si>
+    <t>0.2644±0.0465</t>
+  </si>
+  <si>
+    <t>0.6743±0.0287</t>
+  </si>
+  <si>
+    <t>0.6322±0.0232</t>
+  </si>
+  <si>
+    <t>0.6019±0.0197</t>
+  </si>
+  <si>
+    <t>0.5654±0.0317</t>
+  </si>
+  <si>
+    <t>0.5564±0.0336</t>
+  </si>
+  <si>
+    <t>0.1211±0.0648</t>
+  </si>
+  <si>
+    <t>0.6115±0.0339</t>
+  </si>
+  <si>
+    <t>0.5608±0.0323</t>
+  </si>
+  <si>
+    <t>0.5687±0.0154</t>
+  </si>
+  <si>
+    <t>0.5548±0.0193</t>
+  </si>
+  <si>
+    <t>0.5566±0.0204</t>
+  </si>
+  <si>
+    <t>0.1114±0.0396</t>
+  </si>
+  <si>
+    <t>0.5557±0.0198</t>
+  </si>
+  <si>
+    <t>0.5193±0.0335</t>
+  </si>
+  <si>
+    <t>0.5492±0.0268</t>
+  </si>
+  <si>
+    <t>0.5473±0.0272</t>
+  </si>
+  <si>
+    <t>0.0963±0.0538</t>
+  </si>
+  <si>
+    <t>0.5482±0.0269</t>
+  </si>
+  <si>
+    <t>0.6482±0.016</t>
+  </si>
+  <si>
+    <t>0.6265±0.0189</t>
+  </si>
+  <si>
+    <t>0.5986±0.0338</t>
+  </si>
+  <si>
+    <t>0.2206±0.056</t>
+  </si>
+  <si>
+    <t>0.6619±0.0325</t>
+  </si>
+  <si>
+    <t>0.612±0.0251</t>
+  </si>
+  <si>
+    <t>0.6351±0.0232</t>
+  </si>
+  <si>
+    <t>0.6079±0.0307</t>
+  </si>
+  <si>
+    <t>0.5893±0.032</t>
+  </si>
+  <si>
+    <t>0.1959±0.0614</t>
+  </si>
+  <si>
+    <t>0.668±0.0324</t>
+  </si>
+  <si>
+    <t>0.5984±0.0306</t>
+  </si>
+  <si>
+    <t>0.6527±0.0308</t>
+  </si>
+  <si>
+    <t>0.6332±0.0402</t>
+  </si>
+  <si>
+    <t>0.6099±0.0289</t>
+  </si>
+  <si>
+    <t>0.2413±0.0657</t>
+  </si>
+  <si>
+    <t>0.6642±0.0322</t>
+  </si>
+  <si>
+    <t>0.6211±0.0331</t>
+  </si>
+  <si>
+    <t>0.6446±0.0279</t>
+  </si>
+  <si>
+    <t>0.6216±0.0323</t>
+  </si>
+  <si>
+    <t>0.615±0.0315</t>
+  </si>
+  <si>
+    <t>0.2365±0.0636</t>
+  </si>
+  <si>
+    <t>0.6669±0.0317</t>
+  </si>
+  <si>
+    <t>0.6183±0.0318</t>
+  </si>
+  <si>
+    <t>0.6418±0.0186</t>
+  </si>
+  <si>
+    <t>0.6149±0.0232</t>
+  </si>
+  <si>
+    <t>0.5956±0.0239</t>
+  </si>
+  <si>
+    <t>0.2094±0.0466</t>
+  </si>
+  <si>
+    <t>0.6577±0.028</t>
+  </si>
+  <si>
+    <t>0.6051±0.0232</t>
+  </si>
+  <si>
+    <t>0.643±0.0116</t>
+  </si>
+  <si>
+    <t>0.6167±0.0145</t>
+  </si>
+  <si>
+    <t>0.5983±0.0127</t>
+  </si>
+  <si>
+    <t>0.2142±0.0263</t>
+  </si>
+  <si>
+    <t>0.6442±0.0172</t>
+  </si>
+  <si>
+    <t>0.6074±0.0132</t>
+  </si>
+  <si>
+    <t>0.6492±0.0151</t>
+  </si>
+  <si>
+    <t>0.6264±0.0166</t>
+  </si>
+  <si>
+    <t>0.6176±0.0156</t>
+  </si>
+  <si>
+    <t>0.2438±0.0316</t>
+  </si>
+  <si>
+    <t>0.6787±0.0217</t>
+  </si>
+  <si>
+    <t>0.622±0.0158</t>
+  </si>
+  <si>
+    <t>0.643±0.0188</t>
+  </si>
+  <si>
+    <t>0.621±0.021</t>
+  </si>
+  <si>
+    <t>0.6159±0.0198</t>
+  </si>
+  <si>
+    <t>0.2368±0.0404</t>
+  </si>
+  <si>
+    <t>0.676±0.023</t>
+  </si>
+  <si>
+    <t>0.6184±0.0202</t>
+  </si>
+  <si>
+    <t>0.6346±0.0313</t>
+  </si>
+  <si>
+    <t>0.6131±0.0327</t>
+  </si>
+  <si>
+    <t>0.6091±0.0318</t>
+  </si>
+  <si>
+    <t>0.2221±0.0642</t>
+  </si>
+  <si>
+    <t>0.6631±0.0343</t>
+  </si>
+  <si>
+    <t>0.6111±0.0321</t>
+  </si>
+  <si>
+    <t>0.6122±0.0263</t>
+  </si>
+  <si>
+    <t>0.5735±0.0433</t>
+  </si>
+  <si>
+    <t>0.5562±0.0364</t>
+  </si>
+  <si>
+    <t>0.1278±0.0776</t>
+  </si>
+  <si>
+    <t>0.6115±0.0397</t>
+  </si>
+  <si>
+    <t>0.5646±0.039</t>
+  </si>
+  <si>
+    <t>0.5473±0.0303</t>
+  </si>
+  <si>
+    <t>0.5344±0.0299</t>
+  </si>
+  <si>
+    <t>0.5355±0.0305</t>
+  </si>
+  <si>
+    <t>0.0699±0.0604</t>
+  </si>
+  <si>
+    <t>0.535±0.0302</t>
+  </si>
+  <si>
+    <t>0.5785±0.0214</t>
+  </si>
+  <si>
+    <t>0.5573±0.0197</t>
+  </si>
+  <si>
+    <t>0.557±0.0187</t>
+  </si>
+  <si>
+    <t>0.1143±0.0384</t>
+  </si>
+  <si>
+    <t>0.5571±0.0192</t>
+  </si>
+  <si>
+    <t>0.6573±0.0353</t>
+  </si>
+  <si>
+    <t>0.6358±0.0462</t>
+  </si>
+  <si>
+    <t>0.6027±0.0479</t>
+  </si>
+  <si>
+    <t>0.234±0.0956</t>
+  </si>
+  <si>
+    <t>0.6702±0.0403</t>
+  </si>
+  <si>
+    <t>0.6186±0.0462</t>
+  </si>
+  <si>
+    <t>0.6439±0.0332</t>
+  </si>
+  <si>
+    <t>0.6189±0.044</t>
+  </si>
+  <si>
+    <t>0.5924±0.0348</t>
+  </si>
+  <si>
+    <t>0.2093±0.0777</t>
+  </si>
+  <si>
+    <t>0.6729±0.0279</t>
+  </si>
+  <si>
+    <t>0.6053±0.0389</t>
+  </si>
+  <si>
+    <t>0.6279±0.0158</t>
+  </si>
+  <si>
+    <t>0.5993±0.0331</t>
+  </si>
+  <si>
+    <t>0.5505±0.0166</t>
+  </si>
+  <si>
+    <t>0.1412±0.045</t>
+  </si>
+  <si>
+    <t>0.5355±0.1897</t>
+  </si>
+  <si>
+    <t>0.5737±0.0234</t>
+  </si>
+  <si>
+    <t>0.6222±0.007</t>
+  </si>
+  <si>
+    <t>0.6584±0.0656</t>
+  </si>
+  <si>
+    <t>0.5162±0.0082</t>
+  </si>
+  <si>
+    <t>0.1002±0.0444</t>
+  </si>
+  <si>
+    <t>0.5186±0.0411</t>
+  </si>
+  <si>
+    <t>0.5777±0.0302</t>
+  </si>
+  <si>
+    <t>0.6115±0.0215</t>
+  </si>
+  <si>
+    <t>0.5777±0.0258</t>
+  </si>
+  <si>
+    <t>0.5645±0.0192</t>
+  </si>
+  <si>
+    <t>0.1415±0.0444</t>
+  </si>
+  <si>
+    <t>0.5766±0.0131</t>
+  </si>
+  <si>
+    <t>0.571±0.0223</t>
+  </si>
+  <si>
+    <t>0.6134±0.023</t>
+  </si>
+  <si>
+    <t>0.578±0.0297</t>
+  </si>
+  <si>
+    <t>0.5621±0.0221</t>
+  </si>
+  <si>
+    <t>0.1391±0.051</t>
+  </si>
+  <si>
+    <t>0.5634±0.0239</t>
+  </si>
+  <si>
+    <t>0.5699±0.0257</t>
+  </si>
+  <si>
+    <t>0.6301±0.0154</t>
+  </si>
+  <si>
+    <t>0.5995±0.0243</t>
+  </si>
+  <si>
+    <t>0.5696±0.0139</t>
+  </si>
+  <si>
+    <t>0.1662±0.0356</t>
+  </si>
+  <si>
+    <t>0.6026±0.0125</t>
+  </si>
+  <si>
+    <t>0.5841±0.0182</t>
+  </si>
+  <si>
+    <t>0.61±0.0151</t>
+  </si>
+  <si>
+    <t>0.5717±0.019</t>
+  </si>
+  <si>
+    <t>0.555±0.0134</t>
+  </si>
+  <si>
+    <t>0.1255±0.0318</t>
+  </si>
+  <si>
+    <t>0.5767±0.0132</t>
+  </si>
+  <si>
+    <t>0.5632±0.016</t>
+  </si>
+  <si>
+    <t>0.6215±0.0236</t>
+  </si>
+  <si>
+    <t>0.5902±0.0315</t>
+  </si>
+  <si>
+    <t>0.5667±0.0214</t>
+  </si>
+  <si>
+    <t>0.1545±0.0497</t>
+  </si>
+  <si>
+    <t>0.5768±0.0258</t>
+  </si>
+  <si>
+    <t>0.5781±0.0252</t>
+  </si>
+  <si>
+    <t>0.6243±0.0202</t>
+  </si>
+  <si>
+    <t>0.5912±0.0328</t>
+  </si>
+  <si>
+    <t>0.5561±0.0205</t>
+  </si>
+  <si>
+    <t>0.1426±0.0499</t>
+  </si>
+  <si>
+    <t>0.606±0.031</t>
+  </si>
+  <si>
+    <t>0.573±0.0255</t>
+  </si>
+  <si>
+    <t>0.5322±0.0302</t>
+  </si>
+  <si>
+    <t>0.5029±0.0327</t>
+  </si>
+  <si>
+    <t>0.503±0.0321</t>
+  </si>
+  <si>
+    <t>0.0059±0.0648</t>
+  </si>
+  <si>
+    <t>0.5029±0.0324</t>
+  </si>
+  <si>
+    <t>0.5508±0.0399</t>
+  </si>
+  <si>
+    <t>0.5296±0.043</t>
+  </si>
+  <si>
+    <t>0.53±0.0442</t>
+  </si>
+  <si>
+    <t>0.0597±0.0871</t>
+  </si>
+  <si>
+    <t>0.5291±0.0436</t>
+  </si>
+  <si>
+    <t>0.5298±0.0436</t>
+  </si>
+  <si>
+    <t>0.6272±0.0105</t>
+  </si>
+  <si>
+    <t>0.6356±0.0506</t>
+  </si>
+  <si>
+    <t>0.5302±0.0122</t>
+  </si>
+  <si>
+    <t>0.1251±0.0456</t>
+  </si>
+  <si>
+    <t>0.5584±0.0298</t>
+  </si>
+  <si>
+    <t>0.5775±0.0252</t>
+  </si>
+  <si>
+    <t>0.6224±0.0126</t>
+  </si>
+  <si>
+    <t>0.6053±0.0553</t>
+  </si>
+  <si>
+    <t>0.5289±0.0109</t>
+  </si>
+  <si>
+    <t>0.1093±0.0479</t>
+  </si>
+  <si>
+    <t>0.5552±0.0308</t>
+  </si>
+  <si>
+    <t>0.5639±0.0288</t>
+  </si>
+  <si>
+    <t>0.6382±0.0055</t>
+  </si>
+  <si>
+    <t>0.6226±0.0147</t>
+  </si>
+  <si>
+    <t>0.5587±0.0058</t>
+  </si>
+  <si>
+    <t>0.1694±0.0158</t>
+  </si>
+  <si>
+    <t>0.6177±0.0173</t>
+  </si>
+  <si>
+    <t>0.5889±0.0085</t>
+  </si>
+  <si>
+    <t>0.6141±0.006</t>
+  </si>
+  <si>
+    <t>0.579±0.0641</t>
+  </si>
+  <si>
+    <t>0.5094±0.0074</t>
+  </si>
+  <si>
+    <t>0.0537±0.0417</t>
+  </si>
+  <si>
+    <t>0.5414±0.0287</t>
+  </si>
+  <si>
+    <t>0.5408±0.0322</t>
+  </si>
+  <si>
+    <t>0.6193±0.0185</t>
+  </si>
+  <si>
+    <t>0.5859±0.0239</t>
+  </si>
+  <si>
+    <t>0.5714±0.0226</t>
+  </si>
+  <si>
+    <t>0.1566±0.0462</t>
+  </si>
+  <si>
+    <t>0.6038±0.0175</t>
+  </si>
+  <si>
+    <t>0.5786±0.023</t>
+  </si>
+  <si>
+    <t>0.6174±0.0148</t>
+  </si>
+  <si>
+    <t>0.5823±0.0196</t>
+  </si>
+  <si>
+    <t>0.565±0.0163</t>
+  </si>
+  <si>
+    <t>0.1462±0.0353</t>
+  </si>
+  <si>
+    <t>0.5962±0.0096</t>
+  </si>
+  <si>
+    <t>0.5735±0.0177</t>
+  </si>
+  <si>
+    <t>0.611±0.0104</t>
+  </si>
+  <si>
+    <t>0.5761±0.0121</t>
+  </si>
+  <si>
+    <t>0.5631±0.0098</t>
+  </si>
+  <si>
+    <t>0.1385±0.0213</t>
+  </si>
+  <si>
+    <t>0.5912±0.0184</t>
+  </si>
+  <si>
+    <t>0.5695±0.0107</t>
+  </si>
+  <si>
+    <t>0.6005±0.018</t>
+  </si>
+  <si>
+    <t>0.5652±0.0217</t>
+  </si>
+  <si>
+    <t>0.5566±0.02</t>
+  </si>
+  <si>
+    <t>0.1214±0.0415</t>
+  </si>
+  <si>
+    <t>0.5888±0.0226</t>
+  </si>
+  <si>
+    <t>0.5609±0.0208</t>
+  </si>
+  <si>
+    <t>0.6272±0.0221</t>
+  </si>
+  <si>
+    <t>0.5977±0.0283</t>
+  </si>
+  <si>
+    <t>0.5712±0.0188</t>
+  </si>
+  <si>
+    <t>0.1664±0.0446</t>
+  </si>
+  <si>
+    <t>0.5999±0.0202</t>
+  </si>
+  <si>
+    <t>0.5841±0.0226</t>
+  </si>
+  <si>
+    <t>0.6274±0.0139</t>
+  </si>
+  <si>
+    <t>0.5945±0.0245</t>
+  </si>
+  <si>
+    <t>0.5592±0.0168</t>
+  </si>
+  <si>
+    <t>0.1495±0.0399</t>
+  </si>
+  <si>
+    <t>0.6257±0.0216</t>
+  </si>
+  <si>
+    <t>0.5763±0.0201</t>
+  </si>
+  <si>
+    <t>0.5568±0.0215</t>
+  </si>
+  <si>
+    <t>0.5314±0.024</t>
+  </si>
+  <si>
+    <t>0.5312±0.0239</t>
+  </si>
+  <si>
+    <t>0.0626±0.0479</t>
+  </si>
+  <si>
+    <t>0.5313±0.0239</t>
+  </si>
+  <si>
+    <t>0.5623±0.0211</t>
+  </si>
+  <si>
+    <t>0.5415±0.0228</t>
+  </si>
+  <si>
+    <t>0.542±0.0233</t>
+  </si>
+  <si>
+    <t>0.0835±0.0461</t>
+  </si>
+  <si>
+    <t>0.5423±0.0247</t>
+  </si>
+  <si>
+    <t>0.5418±0.0231</t>
+  </si>
+  <si>
+    <t>0.6251±0.0106</t>
+  </si>
+  <si>
+    <t>0.6035±0.0575</t>
+  </si>
+  <si>
+    <t>0.5285±0.0163</t>
+  </si>
+  <si>
+    <t>0.1085±0.0569</t>
+  </si>
+  <si>
+    <t>0.5863±0.0265</t>
+  </si>
+  <si>
+    <t>0.5628±0.0343</t>
+  </si>
+  <si>
+    <t>0.6255±0.0085</t>
+  </si>
+  <si>
+    <t>0.6094±0.0301</t>
+  </si>
+  <si>
+    <t>0.5323±0.0097</t>
+  </si>
+  <si>
+    <t>0.1186±0.0332</t>
+  </si>
+  <si>
+    <t>0.5842±0.0262</t>
+  </si>
+  <si>
+    <t>0.5681±0.0184</t>
   </si>
 </sst>
 </file>
@@ -4524,7 +5880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE8EA2A-9E9F-440E-AA8B-BE5295D9DA09}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -5112,8 +6468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC63772D-A536-435C-9164-B38BADB6850E}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5666,7 +7022,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="I3" sqref="I3:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5721,60 +7077,2292 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1373</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1376</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="8" spans="1:14" s="3" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1379</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1382</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1383</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1390</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1386</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1391</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1392</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1393</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1383</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1386</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1369</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6D961C-F86D-4B07-BD3E-642EA7591140}">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1679</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1680</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1748</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1750</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1684</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1686</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1752</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1753</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1754</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1755</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1756</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1690</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1691</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1692</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1758</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1759</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1760</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1761</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1762</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1695</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1696</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1697</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1698</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1764</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1765</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1766</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1767</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1768</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1703</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1704</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1770</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1771</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1772</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1773</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1774</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1707</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1708</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1709</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1710</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1776</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1777</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1778</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1779</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1780</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1715</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1782</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1783</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1784</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1785</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1786</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1718</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1721</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1722</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1788</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1789</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1790</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1791</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1792</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1725</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1727</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1794</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1795</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1796</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1797</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1796</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1729</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1730</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1731</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1732</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1733</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1799</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1800</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1801</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1802</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1803</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1736</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1737</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1738</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1739</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1805</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1806</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1807</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1808</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1809</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1741</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1744</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1745</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1811</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1812</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1813</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1814</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1815</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A783E1BD-C980-4FE6-8F21-9C3E6AFF07BE}">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1464</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1468</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1403</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1453</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1470</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1471</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1472</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1473</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1474</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1407</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1408</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1454</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1476</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1477</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1478</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1479</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1480</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1411</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1413</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1455</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1482</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1484</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1485</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1486</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1415</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1417</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1418</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1456</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1488</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1489</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1490</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1491</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1492</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1457</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1494</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1495</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1496</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1497</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1498</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1428</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1458</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1500</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1501</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1502</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1503</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1504</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1459</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1506</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1507</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1508</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1509</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1510</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1436</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1460</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1512</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1513</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1514</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1515</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1514</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1440</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1461</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1517</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1518</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1519</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1520</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1521</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1444</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1523</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1524</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1525</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1526</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1527</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1449</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1451</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1463</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1529</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1530</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1531</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1532</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1533</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818A544D-7051-41A3-A918-FE8166F9DF19}">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1537</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1538</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1539</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1605</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1606</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1607</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1608</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1609</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1545</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1546</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1611</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1613</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1614</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1615</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1549</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1550</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1552</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1617</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1618</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1619</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1620</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1621</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1555</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1556</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1557</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1558</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1623</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1624</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1625</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1626</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1627</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1561</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1563</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1564</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1629</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1630</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1631</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1632</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1633</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1566</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1567</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1568</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1569</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1635</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1636</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1637</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1638</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1639</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1572</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1573</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1574</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1576</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1641</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1642</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1643</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1644</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1645</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1582</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1647</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1648</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1649</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1650</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1651</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1584</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1585</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1586</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1585</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1587</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1653</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1654</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1655</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1656</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1655</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1589</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1590</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1591</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1590</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1592</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1658</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1659</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1660</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1661</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1660</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1594</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1595</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1596</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1597</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1598</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1663</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1664</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1665</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1666</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1667</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1600</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1601</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1602</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1603</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1604</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1669</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1670</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1671</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1672</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1673</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1674</v>
       </c>
     </row>
     <row r="16" spans="1:14">

</xml_diff>